<commit_message>
changed the way how to generate excel file
</commit_message>
<xml_diff>
--- a/InputSample.xlsx
+++ b/InputSample.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="32">
   <si>
     <t>Iterations</t>
   </si>
@@ -31,18 +31,12 @@
     <t>Type</t>
   </si>
   <si>
-    <t>Length</t>
-  </si>
-  <si>
     <t>Pattern</t>
   </si>
   <si>
     <t>String</t>
   </si>
   <si>
-    <t>Test %d</t>
-  </si>
-  <si>
     <t>Float</t>
   </si>
   <si>
@@ -58,20 +52,71 @@
     <t>Integer</t>
   </si>
   <si>
-    <t>%10d</t>
-  </si>
-  <si>
     <t>Output file name</t>
   </si>
   <si>
     <t>outputtest.xlsx</t>
+  </si>
+  <si>
+    <t>Generate</t>
+  </si>
+  <si>
+    <t>y</t>
+  </si>
+  <si>
+    <t>[a-zA-Z]{10}</t>
+  </si>
+  <si>
+    <t>Test [0-9]{10}</t>
+  </si>
+  <si>
+    <t>[0-9]{10}</t>
+  </si>
+  <si>
+    <t>[0]{5}[0-9]{5}</t>
+  </si>
+  <si>
+    <t>Username</t>
+  </si>
+  <si>
+    <t>Some text and numberic id</t>
+  </si>
+  <si>
+    <t>Float number</t>
+  </si>
+  <si>
+    <t>Number with leading zeros</t>
+  </si>
+  <si>
+    <t>Positive 10 digit integer</t>
+  </si>
+  <si>
+    <t>Just string without generation</t>
+  </si>
+  <si>
+    <t>n</t>
+  </si>
+  <si>
+    <t>My String</t>
+  </si>
+  <si>
+    <t>Float pattern</t>
+  </si>
+  <si>
+    <t>[0-9]{2}[.][0-9]{1,5}</t>
+  </si>
+  <si>
+    <t>Date forward</t>
+  </si>
+  <si>
+    <t>19/12/2015</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="3">
+  <fonts count="4">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -85,6 +130,11 @@
       <b/>
       <sz val="10"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -101,7 +151,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -157,11 +207,31 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -170,6 +240,14 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -464,13 +542,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D9"/>
+  <dimension ref="A1:D14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
+  <cols>
+    <col min="1" max="1" width="23.7109375" customWidth="1"/>
+    <col min="4" max="4" width="18.42578125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="15.75" customHeight="1">
       <c r="A1" s="1" t="s">
@@ -490,10 +572,10 @@
     </row>
     <row r="3" spans="1:4" ht="15.75" customHeight="1">
       <c r="A3" s="7" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="15.75" customHeight="1">
@@ -504,75 +586,152 @@
         <v>4</v>
       </c>
       <c r="C4" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D4" s="2" t="s">
+    </row>
+    <row r="5" spans="1:4" ht="15.75" customHeight="1">
+      <c r="A5" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B5" s="4" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" ht="15.75" customHeight="1">
-      <c r="A5" s="3">
-        <v>1</v>
-      </c>
-      <c r="B5" s="4" t="s">
+      <c r="C5" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D5" s="11" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="15.75" customHeight="1">
+      <c r="A6" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D6" s="12" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="15.75" customHeight="1">
+      <c r="A7" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="B7" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="4">
+      <c r="C7" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D7" s="12" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="15.75" customHeight="1">
+      <c r="A8" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D8" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="D5" s="5"/>
-    </row>
-    <row r="6" spans="1:4" ht="15.75" customHeight="1">
-      <c r="A6" s="6">
-        <v>2</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C6" s="4">
-        <v>10</v>
-      </c>
-      <c r="D6" s="4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" ht="15.75" customHeight="1">
-      <c r="A7" s="6">
-        <v>3</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C7" s="5"/>
-      <c r="D7" s="4" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" ht="15.75" customHeight="1">
-      <c r="A8" s="6">
-        <v>4</v>
-      </c>
-      <c r="B8" s="4" t="s">
+    </row>
+    <row r="9" spans="1:4" ht="15.75" customHeight="1">
+      <c r="A9" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D9" s="11" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="15.75" customHeight="1">
+      <c r="A10" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="C8" s="5"/>
-      <c r="D8" s="4" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" ht="15.75" customHeight="1">
-      <c r="A9" s="6">
-        <v>5</v>
-      </c>
-      <c r="B9" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="C9" s="5"/>
-      <c r="D9" s="4" t="s">
-        <v>14</v>
+      <c r="B10" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D10" s="13"/>
+    </row>
+    <row r="11" spans="1:4" ht="15.75" customHeight="1">
+      <c r="A11" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="B11" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="C11" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="D11" s="12" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="15.75" customHeight="1">
+      <c r="A12" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="B12" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="C12" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="D12" s="14" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="15.75" customHeight="1">
+      <c r="A13" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="B13" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="C13" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="D13" s="14" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="15.75" customHeight="1">
+      <c r="A14" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="B14" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="C14" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="D14" s="15" t="s">
+        <v>31</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added string and numberic ranges
</commit_message>
<xml_diff>
--- a/InputSample.xlsx
+++ b/InputSample.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="39">
   <si>
     <t>Iterations</t>
   </si>
@@ -40,9 +40,6 @@
     <t>Float</t>
   </si>
   <si>
-    <t>%.05f</t>
-  </si>
-  <si>
     <t>Date</t>
   </si>
   <si>
@@ -110,13 +107,37 @@
   </si>
   <si>
     <t>19/12/2015</t>
+  </si>
+  <si>
+    <t>Range</t>
+  </si>
+  <si>
+    <t>M,F</t>
+  </si>
+  <si>
+    <t>Gender selection from range</t>
+  </si>
+  <si>
+    <t>Locale selection from range</t>
+  </si>
+  <si>
+    <t>US, UK, EU</t>
+  </si>
+  <si>
+    <t>Number range</t>
+  </si>
+  <si>
+    <t>NumberRange</t>
+  </si>
+  <si>
+    <t>-5:10</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -136,6 +157,12 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -151,7 +178,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -227,11 +254,22 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -248,6 +286,10 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -542,15 +584,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D14"/>
+  <dimension ref="A1:D17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="23.7109375" customWidth="1"/>
+    <col min="1" max="1" width="28.28515625" customWidth="1"/>
     <col min="4" max="4" width="18.42578125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -572,10 +614,10 @@
     </row>
     <row r="3" spans="1:4" ht="15.75" customHeight="1">
       <c r="A3" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" s="7" t="s">
         <v>12</v>
-      </c>
-      <c r="B3" s="7" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="15.75" customHeight="1">
@@ -586,7 +628,7 @@
         <v>4</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>5</v>
@@ -594,140 +636,180 @@
     </row>
     <row r="5" spans="1:4" ht="15.75" customHeight="1">
       <c r="A5" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>6</v>
       </c>
       <c r="C5" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D5" s="11" t="s">
         <v>15</v>
-      </c>
-      <c r="D5" s="11" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="15.75" customHeight="1">
       <c r="A6" s="6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B6" s="4" t="s">
         <v>6</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D6" s="12" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="15.75" customHeight="1">
       <c r="A7" s="6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B7" s="4" t="s">
         <v>7</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="D7" s="12" t="s">
-        <v>8</v>
-      </c>
+        <v>14</v>
+      </c>
+      <c r="D7" s="12"/>
     </row>
     <row r="8" spans="1:4" ht="15.75" customHeight="1">
       <c r="A8" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D8" s="12" t="s">
         <v>9</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C8" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="D8" s="12" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="15.75" customHeight="1">
       <c r="A9" s="6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B9" s="4" t="s">
         <v>6</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D9" s="11" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="15.75" customHeight="1">
       <c r="A10" s="6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D10" s="13"/>
     </row>
     <row r="11" spans="1:4" ht="15.75" customHeight="1">
       <c r="A11" s="8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B11" s="9" t="s">
         <v>6</v>
       </c>
       <c r="C11" s="9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D11" s="12" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="15.75" customHeight="1">
       <c r="A12" s="8" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B12" s="9" t="s">
         <v>6</v>
       </c>
       <c r="C12" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="D12" s="14" t="s">
         <v>26</v>
-      </c>
-      <c r="D12" s="14" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="15.75" customHeight="1">
       <c r="A13" s="8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B13" s="9" t="s">
         <v>6</v>
       </c>
       <c r="C13" s="9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D13" s="14" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="15.75" customHeight="1">
       <c r="A14" s="8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B14" s="9" t="s">
         <v>6</v>
       </c>
       <c r="C14" s="9" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D14" s="15" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="15.75" customHeight="1">
+      <c r="A15" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="B15" s="9" t="s">
         <v>31</v>
+      </c>
+      <c r="C15" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="D15" s="17" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="15.75" customHeight="1">
+      <c r="A16" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="B16" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="C16" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="D16" s="17" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="15.75" customHeight="1">
+      <c r="A17" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="B17" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="C17" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="D17" s="19" t="s">
+        <v>38</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added date range generator
</commit_message>
<xml_diff>
--- a/InputSample.xlsx
+++ b/InputSample.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="42">
   <si>
     <t>Iterations</t>
   </si>
@@ -131,6 +131,15 @@
   </si>
   <si>
     <t>-5:10</t>
+  </si>
+  <si>
+    <t>Date range</t>
+  </si>
+  <si>
+    <t>DateRange</t>
+  </si>
+  <si>
+    <t>dd/MM/yyyy:10/05/1965:25/12/1965</t>
   </si>
 </sst>
 </file>
@@ -269,7 +278,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -290,6 +299,7 @@
     <xf numFmtId="49" fontId="3" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="4" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -584,16 +594,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D17"/>
+  <dimension ref="A1:D18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="28.28515625" customWidth="1"/>
-    <col min="4" max="4" width="18.42578125" customWidth="1"/>
+    <col min="4" max="4" width="33" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="15.75" customHeight="1">
@@ -812,6 +822,20 @@
         <v>38</v>
       </c>
     </row>
+    <row r="18" spans="1:4" ht="15.75" customHeight="1">
+      <c r="A18" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="B18" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="C18" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="D18" s="20" t="s">
+        <v>41</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
added bat files as sample of usage
</commit_message>
<xml_diff>
--- a/InputSample.xlsx
+++ b/InputSample.xlsx
@@ -600,7 +600,7 @@
   <dimension ref="A1:D19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
@@ -614,7 +614,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1">
-        <v>1048575</v>
+        <v>30000</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="15.75" customHeight="1">

</xml_diff>

<commit_message>
added possibility define types for generated cells
</commit_message>
<xml_diff>
--- a/InputSample.xlsx
+++ b/InputSample.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="42">
   <si>
     <t>Iterations</t>
   </si>
@@ -41,9 +41,6 @@
   </si>
   <si>
     <t>Date</t>
-  </si>
-  <si>
-    <t>dd/MM/YY</t>
   </si>
   <si>
     <t>Integer</t>
@@ -281,7 +278,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -303,6 +300,8 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="4" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -614,7 +613,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1">
-        <v>30000</v>
+        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="15.75" customHeight="1">
@@ -627,18 +626,18 @@
     </row>
     <row r="3" spans="1:4" ht="15.75" customHeight="1">
       <c r="A3" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" s="7" t="s">
         <v>11</v>
-      </c>
-      <c r="B3" s="7" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="15.75" customHeight="1">
       <c r="A4" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B4" s="7">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="15.75" customHeight="1">
@@ -649,7 +648,7 @@
         <v>4</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>5</v>
@@ -657,41 +656,41 @@
     </row>
     <row r="6" spans="1:4" ht="15.75" customHeight="1">
       <c r="A6" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B6" s="4" t="s">
         <v>6</v>
       </c>
       <c r="C6" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D6" s="11" t="s">
         <v>14</v>
-      </c>
-      <c r="D6" s="11" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="15.75" customHeight="1">
       <c r="A7" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B7" s="4" t="s">
         <v>6</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D7" s="12" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="15.75" customHeight="1">
       <c r="A8" s="6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B8" s="4" t="s">
         <v>7</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D8" s="12"/>
     </row>
@@ -703,148 +702,146 @@
         <v>8</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="D9" s="12" t="s">
-        <v>9</v>
-      </c>
+        <v>13</v>
+      </c>
+      <c r="D9" s="12"/>
     </row>
     <row r="10" spans="1:4" ht="15.75" customHeight="1">
       <c r="A10" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="B10" s="4" t="s">
-        <v>6</v>
+        <v>21</v>
+      </c>
+      <c r="B10" s="21" t="s">
+        <v>9</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D10" s="11" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="15.75" customHeight="1">
       <c r="A11" s="6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D11" s="13"/>
     </row>
     <row r="12" spans="1:4" ht="15.75" customHeight="1">
       <c r="A12" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="B12" s="9" t="s">
-        <v>6</v>
+        <v>22</v>
+      </c>
+      <c r="B12" s="22" t="s">
+        <v>9</v>
       </c>
       <c r="C12" s="9" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D12" s="12" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="15.75" customHeight="1">
       <c r="A13" s="8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B13" s="9" t="s">
         <v>6</v>
       </c>
       <c r="C13" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="D13" s="14" t="s">
         <v>25</v>
-      </c>
-      <c r="D13" s="14" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="15.75" customHeight="1">
       <c r="A14" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="B14" s="22" t="s">
+        <v>7</v>
+      </c>
+      <c r="C14" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="D14" s="14" t="s">
         <v>27</v>
-      </c>
-      <c r="B14" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="C14" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="D14" s="14" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="15.75" customHeight="1">
       <c r="A15" s="8" t="s">
-        <v>41</v>
-      </c>
-      <c r="B15" s="9" t="s">
-        <v>6</v>
+        <v>40</v>
+      </c>
+      <c r="B15" s="22" t="s">
+        <v>8</v>
       </c>
       <c r="C15" s="9" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D15" s="15" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="15.75" customHeight="1">
       <c r="A16" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B16" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="C16" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="D16" s="17" t="s">
         <v>30</v>
-      </c>
-      <c r="C16" s="16" t="s">
-        <v>14</v>
-      </c>
-      <c r="D16" s="17" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="15.75" customHeight="1">
       <c r="A17" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="B17" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="C17" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="D17" s="17" t="s">
         <v>33</v>
-      </c>
-      <c r="B17" s="9" t="s">
-        <v>30</v>
-      </c>
-      <c r="C17" s="16" t="s">
-        <v>14</v>
-      </c>
-      <c r="D17" s="17" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="15.75" customHeight="1">
       <c r="A18" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="B18" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="B18" s="9" t="s">
+      <c r="C18" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="D18" s="19" t="s">
         <v>36</v>
-      </c>
-      <c r="C18" s="18" t="s">
-        <v>14</v>
-      </c>
-      <c r="D18" s="19" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="15.75" customHeight="1">
       <c r="A19" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="B19" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="B19" s="9" t="s">
+      <c r="C19" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="D19" s="20" t="s">
         <v>39</v>
-      </c>
-      <c r="C19" s="18" t="s">
-        <v>14</v>
-      </c>
-      <c r="D19" s="20" t="s">
-        <v>40</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added sequental number generation
</commit_message>
<xml_diff>
--- a/InputSample.xlsx
+++ b/InputSample.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\devtools\mywork\filegen-repo\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="510" yWindow="525" windowWidth="20775" windowHeight="11445"/>
   </bookViews>
@@ -14,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="45">
   <si>
     <t>Iterations</t>
   </si>
@@ -49,104 +54,113 @@
     <t>Output file name</t>
   </si>
   <si>
+    <t>Generate</t>
+  </si>
+  <si>
+    <t>y</t>
+  </si>
+  <si>
+    <t>[a-zA-Z]{10}</t>
+  </si>
+  <si>
+    <t>Test [0-9]{10}</t>
+  </si>
+  <si>
+    <t>[0-9]{10}</t>
+  </si>
+  <si>
+    <t>[0]{5}[0-9]{5}</t>
+  </si>
+  <si>
+    <t>Username</t>
+  </si>
+  <si>
+    <t>Some text and numberic id</t>
+  </si>
+  <si>
+    <t>Float number</t>
+  </si>
+  <si>
+    <t>Number with leading zeros</t>
+  </si>
+  <si>
+    <t>Positive 10 digit integer</t>
+  </si>
+  <si>
+    <t>Just string without generation</t>
+  </si>
+  <si>
+    <t>n</t>
+  </si>
+  <si>
+    <t>My String</t>
+  </si>
+  <si>
+    <t>Float pattern</t>
+  </si>
+  <si>
+    <t>[0-9]{2}[.][0-9]{1,5}</t>
+  </si>
+  <si>
+    <t>19/12/2015</t>
+  </si>
+  <si>
+    <t>Range</t>
+  </si>
+  <si>
+    <t>M,F</t>
+  </si>
+  <si>
+    <t>Gender selection from range</t>
+  </si>
+  <si>
+    <t>Locale selection from range</t>
+  </si>
+  <si>
+    <t>US, UK, EU</t>
+  </si>
+  <si>
+    <t>Number range</t>
+  </si>
+  <si>
+    <t>NumberRange</t>
+  </si>
+  <si>
+    <t>-5:10</t>
+  </si>
+  <si>
+    <t>Date range</t>
+  </si>
+  <si>
+    <t>DateRange</t>
+  </si>
+  <si>
+    <t>dd/MM/yyyy:10/05/1965:25/12/1967</t>
+  </si>
+  <si>
+    <t>Date without generation</t>
+  </si>
+  <si>
+    <t>Sheet count:</t>
+  </si>
+  <si>
+    <t>Auto number</t>
+  </si>
+  <si>
+    <t>AutoNumber</t>
+  </si>
+  <si>
+    <t>5</t>
+  </si>
+  <si>
     <t>outputtest.xlsx</t>
-  </si>
-  <si>
-    <t>Generate</t>
-  </si>
-  <si>
-    <t>y</t>
-  </si>
-  <si>
-    <t>[a-zA-Z]{10}</t>
-  </si>
-  <si>
-    <t>Test [0-9]{10}</t>
-  </si>
-  <si>
-    <t>[0-9]{10}</t>
-  </si>
-  <si>
-    <t>[0]{5}[0-9]{5}</t>
-  </si>
-  <si>
-    <t>Username</t>
-  </si>
-  <si>
-    <t>Some text and numberic id</t>
-  </si>
-  <si>
-    <t>Float number</t>
-  </si>
-  <si>
-    <t>Number with leading zeros</t>
-  </si>
-  <si>
-    <t>Positive 10 digit integer</t>
-  </si>
-  <si>
-    <t>Just string without generation</t>
-  </si>
-  <si>
-    <t>n</t>
-  </si>
-  <si>
-    <t>My String</t>
-  </si>
-  <si>
-    <t>Float pattern</t>
-  </si>
-  <si>
-    <t>[0-9]{2}[.][0-9]{1,5}</t>
-  </si>
-  <si>
-    <t>19/12/2015</t>
-  </si>
-  <si>
-    <t>Range</t>
-  </si>
-  <si>
-    <t>M,F</t>
-  </si>
-  <si>
-    <t>Gender selection from range</t>
-  </si>
-  <si>
-    <t>Locale selection from range</t>
-  </si>
-  <si>
-    <t>US, UK, EU</t>
-  </si>
-  <si>
-    <t>Number range</t>
-  </si>
-  <si>
-    <t>NumberRange</t>
-  </si>
-  <si>
-    <t>-5:10</t>
-  </si>
-  <si>
-    <t>Date range</t>
-  </si>
-  <si>
-    <t>DateRange</t>
-  </si>
-  <si>
-    <t>dd/MM/yyyy:10/05/1965:25/12/1967</t>
-  </si>
-  <si>
-    <t>Date without generation</t>
-  </si>
-  <si>
-    <t>Sheet count:</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="5">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -308,6 +322,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -354,7 +376,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -386,9 +408,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -420,6 +443,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -595,28 +619,28 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D19"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="28.28515625" customWidth="1"/>
     <col min="4" max="4" width="33" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15.75" customHeight="1">
+    <row r="1" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" ht="15.75" customHeight="1">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -624,23 +648,23 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="15.75" customHeight="1">
+    <row r="3" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="7" t="s">
         <v>10</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" ht="15.75" customHeight="1">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="7" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B4" s="7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" ht="15.75" customHeight="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>3</v>
       </c>
@@ -648,53 +672,53 @@
         <v>4</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="15.75" customHeight="1">
+    <row r="6" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B6" s="4" t="s">
         <v>6</v>
       </c>
       <c r="C6" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D6" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="D6" s="11" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" ht="15.75" customHeight="1">
+    </row>
+    <row r="7" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B7" s="4" t="s">
         <v>6</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D7" s="12" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" ht="15.75" customHeight="1">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B8" s="4" t="s">
         <v>7</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D8" s="12"/>
     </row>
-    <row r="9" spans="1:4" ht="15.75" customHeight="1">
+    <row r="9" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="10" t="s">
         <v>8</v>
       </c>
@@ -702,25 +726,25 @@
         <v>8</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D9" s="12"/>
     </row>
-    <row r="10" spans="1:4" ht="15.75" customHeight="1">
+    <row r="10" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B10" s="21" t="s">
         <v>9</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D10" s="11" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" ht="15.75" customHeight="1">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="6" t="s">
         <v>9</v>
       </c>
@@ -728,120 +752,134 @@
         <v>9</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D11" s="13"/>
     </row>
-    <row r="12" spans="1:4" ht="15.75" customHeight="1">
+    <row r="12" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B12" s="22" t="s">
         <v>9</v>
       </c>
       <c r="C12" s="9" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D12" s="12" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" ht="15.75" customHeight="1">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B13" s="9" t="s">
         <v>6</v>
       </c>
       <c r="C13" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="D13" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="D13" s="14" t="s">
+    </row>
+    <row r="14" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="8" t="s">
         <v>25</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" ht="15.75" customHeight="1">
-      <c r="A14" s="8" t="s">
-        <v>26</v>
       </c>
       <c r="B14" s="22" t="s">
         <v>7</v>
       </c>
       <c r="C14" s="9" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D14" s="14" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" ht="15.75" customHeight="1">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="8" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B15" s="22" t="s">
         <v>8</v>
       </c>
       <c r="C15" s="9" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D15" s="15" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="B16" s="9" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" ht="15.75" customHeight="1">
-      <c r="A16" s="8" t="s">
+      <c r="C16" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="D16" s="17" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="B16" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="C16" s="16" t="s">
-        <v>13</v>
-      </c>
-      <c r="D16" s="17" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" ht="15.75" customHeight="1">
-      <c r="A17" s="8" t="s">
+      <c r="B17" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="C17" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="D17" s="17" t="s">
         <v>32</v>
       </c>
-      <c r="B17" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="C17" s="16" t="s">
-        <v>13</v>
-      </c>
-      <c r="D17" s="17" t="s">
+    </row>
+    <row r="18" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="8" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" ht="15.75" customHeight="1">
-      <c r="A18" s="8" t="s">
+      <c r="B18" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="B18" s="9" t="s">
+      <c r="C18" s="18" t="s">
+        <v>12</v>
+      </c>
+      <c r="D18" s="19" t="s">
         <v>35</v>
       </c>
-      <c r="C18" s="18" t="s">
-        <v>13</v>
-      </c>
-      <c r="D18" s="19" t="s">
+    </row>
+    <row r="19" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="8" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" ht="15.75" customHeight="1">
-      <c r="A19" s="8" t="s">
+      <c r="B19" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="B19" s="9" t="s">
+      <c r="C19" s="18" t="s">
+        <v>12</v>
+      </c>
+      <c r="D19" s="20" t="s">
         <v>38</v>
       </c>
-      <c r="C19" s="18" t="s">
-        <v>13</v>
-      </c>
-      <c r="D19" s="20" t="s">
-        <v>39</v>
+    </row>
+    <row r="20" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="B20" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="C20" s="18" t="s">
+        <v>12</v>
+      </c>
+      <c r="D20" s="20" t="s">
+        <v>43</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added draft implementation of special sequence generator
</commit_message>
<xml_diff>
--- a/InputSample.xlsx
+++ b/InputSample.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="48">
   <si>
     <t>Iterations</t>
   </si>
@@ -154,6 +154,15 @@
   </si>
   <si>
     <t>outputtest.xlsx</t>
+  </si>
+  <si>
+    <t>Sequence generator</t>
+  </si>
+  <si>
+    <t>Sequence</t>
+  </si>
+  <si>
+    <t>ALP01_5_[SEQ(4,3,FAIL)] GEN</t>
   </si>
 </sst>
 </file>
@@ -620,10 +629,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D20"/>
+  <dimension ref="A1:D21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -882,6 +891,20 @@
         <v>43</v>
       </c>
     </row>
+    <row r="21" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="B21" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="C21" s="18" t="s">
+        <v>12</v>
+      </c>
+      <c r="D21" s="20" t="s">
+        <v>47</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
implemented reset functionality for sequence
</commit_message>
<xml_diff>
--- a/InputSample.xlsx
+++ b/InputSample.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="49">
   <si>
     <t>Iterations</t>
   </si>
@@ -163,6 +163,9 @@
   </si>
   <si>
     <t>ALP01_5_[SEQ(4,3,FAIL)] GEN</t>
+  </si>
+  <si>
+    <t>[SEQ(4,1,RESTART)]</t>
   </si>
 </sst>
 </file>
@@ -629,10 +632,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D21"/>
+  <dimension ref="A1:D22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -905,6 +908,20 @@
         <v>47</v>
       </c>
     </row>
+    <row r="22" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="B22" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="C22" s="18" t="s">
+        <v>12</v>
+      </c>
+      <c r="D22" s="20" t="s">
+        <v>48</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
fixed leading zero numbers
</commit_message>
<xml_diff>
--- a/InputSample.xlsx
+++ b/InputSample.xlsx
@@ -634,8 +634,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>